<commit_message>
添加几个函数：zxparam_check zxparam_get zxparam_assign zxAsk zxDial。和一些小调整
</commit_message>
<xml_diff>
--- a/API.xlsx
+++ b/API.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="99">
   <si>
     <t>根据时间戳，返回格式化后的日期</t>
   </si>
@@ -866,6 +866,69 @@
   </si>
   <si>
     <t>检测数组是否包含指定值，返回boolean【完全可以被some方法取代】</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Array对象.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>convert_to_treedata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(param)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>把平级的arr转换成嵌套的树形arr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>before_idkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>before_parentkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>after_childkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原始数据中的id的key，默认为"id"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原始数据中的parentId的key，默认为"parentId"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成数据中的child的key，默认为"child"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>具体用法可以看 \EXAMPLE\13 zxTreetable.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arr.convert_to_treedata({ before_idkey: "deptId" })</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -873,7 +936,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -927,6 +990,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -954,7 +1025,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1040,11 +1111,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1080,46 +1162,77 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1468,10 +1581,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1492,18 +1605,18 @@
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="B3" s="31" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="29" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -1514,10 +1627,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="32"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="8" t="s">
         <v>45</v>
       </c>
@@ -1526,18 +1639,18 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1548,9 +1661,9 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="22" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="34" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1558,24 +1671,24 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="22"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="22"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="31" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1586,8 +1699,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1596,17 +1709,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1618,8 +1731,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1630,8 +1743,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="8" t="s">
         <v>46</v>
       </c>
@@ -1640,8 +1753,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="8" t="s">
         <v>23</v>
       </c>
@@ -1650,17 +1763,17 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="10" t="s">
         <v>26</v>
       </c>
@@ -1672,7 +1785,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="11" t="s">
         <v>32</v>
       </c>
@@ -1684,17 +1797,17 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="7" t="s">
         <v>26</v>
       </c>
@@ -1706,17 +1819,17 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="18"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="10" t="s">
         <v>26</v>
       </c>
@@ -1728,17 +1841,17 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="7" t="s">
         <v>26</v>
       </c>
@@ -1767,21 +1880,21 @@
       <c r="A36" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="27"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="22"/>
     </row>
     <row r="45" spans="1:4" s="12" customFormat="1" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A45" s="19" t="s">
@@ -1795,159 +1908,228 @@
       <c r="A46" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="B46" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="27"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="22"/>
     </row>
     <row r="47" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="29"/>
-      <c r="D47" s="30"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28"/>
     </row>
     <row r="48" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B48" s="25" t="s">
+      <c r="B48" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="26"/>
-      <c r="D48" s="27"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="22"/>
     </row>
     <row r="49" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B49" s="28" t="s">
+      <c r="B49" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="29"/>
-      <c r="D49" s="30"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="28"/>
     </row>
     <row r="50" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="25" t="s">
+      <c r="B50" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="26"/>
-      <c r="D50" s="27"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="22"/>
     </row>
     <row r="51" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="29"/>
-      <c r="D51" s="30"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="28"/>
     </row>
     <row r="52" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="25" t="s">
+      <c r="B52" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="26"/>
-      <c r="D52" s="27"/>
-    </row>
-    <row r="53" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="15"/>
-      <c r="B53" s="15"/>
-    </row>
-    <row r="54" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="15"/>
-      <c r="B54" s="15"/>
-    </row>
-    <row r="55" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
-      <c r="A56" s="19" t="s">
+      <c r="C52" s="21"/>
+      <c r="D52" s="22"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="48"/>
+      <c r="B54" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="48"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="48"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="48"/>
+      <c r="B57" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="43"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
+    </row>
+    <row r="60" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
+      <c r="A61" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B56" s="19"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="24" t="s">
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="38"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="B57" s="23" t="s">
+      <c r="B62" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="23"/>
-      <c r="D57" s="23"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="24"/>
-      <c r="B58" s="23" t="s">
+      <c r="C62" s="45"/>
+      <c r="D62" s="46"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="30"/>
+      <c r="B63" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="18" t="s">
+      <c r="C63" s="45"/>
+      <c r="D63" s="46"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B64" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="18"/>
-      <c r="B60" s="17" t="s">
+      <c r="C64" s="41"/>
+      <c r="D64" s="40"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="43"/>
+      <c r="B65" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C60" s="17"/>
-      <c r="D60" s="2" t="s">
+      <c r="C65" s="40"/>
+      <c r="D65" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
+    <row r="66" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="23" t="s">
+      <c r="B66" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
-    </row>
-    <row r="62" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="10" t="s">
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+    </row>
+    <row r="67" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B67" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-    </row>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+    </row>
+    <row r="71" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
+  <mergeCells count="44">
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:C65"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:B4"/>
@@ -1957,28 +2139,19 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="A53:A58"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>